<commit_message>
Correccion de errores minimos
</commit_message>
<xml_diff>
--- a/src/main/java/IO/data/entrada.xlsx
+++ b/src/main/java/IO/data/entrada.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hml10\IdeaProjects\AlgoritmoGenetico3DBinPackingHeterogeneo\src\main\java\IO\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{767DD603-3E69-4348-84B5-165A42FCCB93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B3817D9-C41C-488B-B51E-AE0BF34ABBF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7896" yWindow="3792" windowWidth="11784" windowHeight="8964" xr2:uid="{9F69F4AE-1FF3-4506-8F1F-CF6B9B237AA2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{9F69F4AE-1FF3-4506-8F1F-CF6B9B237AA2}"/>
   </bookViews>
   <sheets>
     <sheet name="PAQUETES" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
   <si>
     <t>ID</t>
   </si>
@@ -62,16 +62,85 @@
   </si>
   <si>
     <t>LIMITE DE PESO</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>P4</t>
+  </si>
+  <si>
+    <t>P5</t>
+  </si>
+  <si>
+    <t>P6</t>
+  </si>
+  <si>
+    <t>P7</t>
+  </si>
+  <si>
+    <t>P8</t>
+  </si>
+  <si>
+    <t>P9</t>
+  </si>
+  <si>
+    <t>P10</t>
+  </si>
+  <si>
+    <t>P11</t>
+  </si>
+  <si>
+    <t>P12</t>
+  </si>
+  <si>
+    <t>P13</t>
+  </si>
+  <si>
+    <t>P14</t>
+  </si>
+  <si>
+    <t>P15</t>
+  </si>
+  <si>
+    <t>P16</t>
+  </si>
+  <si>
+    <t>P17</t>
+  </si>
+  <si>
+    <t>P18</t>
+  </si>
+  <si>
+    <t>P19</t>
+  </si>
+  <si>
+    <t>P20</t>
+  </si>
+  <si>
+    <t>P21</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -97,8 +166,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -413,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDFBB69F-B6DC-4AE7-ABC1-EA1EEDB45E5A}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C34" sqref="A26:C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -424,7 +494,7 @@
     <col min="6" max="6" width="18.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -447,17 +517,511 @@
         <v>6</v>
       </c>
     </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>9</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
+      <c r="G2">
+        <v>7</v>
+      </c>
+      <c r="H2">
+        <v>3</v>
+      </c>
+      <c r="I2">
+        <v>10</v>
+      </c>
+      <c r="J2">
+        <v>10</v>
+      </c>
+      <c r="K2">
+        <v>7</v>
+      </c>
+      <c r="L2">
+        <v>3</v>
+      </c>
+      <c r="M2">
+        <v>3</v>
+      </c>
+      <c r="N2">
+        <v>7</v>
+      </c>
+      <c r="O2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>6</v>
+      </c>
+      <c r="E3">
+        <v>7</v>
+      </c>
+      <c r="F3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>8</v>
+      </c>
+      <c r="F4">
+        <v>8</v>
+      </c>
+      <c r="G4">
+        <v>10</v>
+      </c>
+      <c r="H4">
+        <v>9</v>
+      </c>
+      <c r="I4">
+        <v>5</v>
+      </c>
+      <c r="J4">
+        <v>9</v>
+      </c>
+      <c r="K4">
+        <v>5</v>
+      </c>
+      <c r="L4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>6</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>8</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>10</v>
+      </c>
+      <c r="D7">
+        <v>8</v>
+      </c>
+      <c r="E7">
+        <v>8</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <v>9</v>
+      </c>
+      <c r="E8">
+        <v>9</v>
+      </c>
+      <c r="F8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>7</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="F9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>9</v>
+      </c>
+      <c r="D10">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <v>10</v>
+      </c>
+      <c r="F11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12">
+        <v>6</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+      <c r="F12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>6</v>
+      </c>
+      <c r="D13">
+        <v>10</v>
+      </c>
+      <c r="E13">
+        <v>5</v>
+      </c>
+      <c r="F13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>6</v>
+      </c>
+      <c r="D14">
+        <v>6</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15">
+        <v>10</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
+      </c>
+      <c r="D15">
+        <v>5</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="F15">
+        <v>3</v>
+      </c>
+      <c r="G15">
+        <v>4</v>
+      </c>
+      <c r="H15">
+        <v>10</v>
+      </c>
+      <c r="I15">
+        <v>5</v>
+      </c>
+      <c r="J15">
+        <v>5</v>
+      </c>
+      <c r="K15">
+        <v>10</v>
+      </c>
+      <c r="L15">
+        <v>4</v>
+      </c>
+      <c r="M15">
+        <v>5</v>
+      </c>
+      <c r="N15">
+        <v>4</v>
+      </c>
+      <c r="O15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16">
+        <v>6</v>
+      </c>
+      <c r="C16">
+        <v>10</v>
+      </c>
+      <c r="D16">
+        <v>8</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17">
+        <v>7</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17">
+        <v>3</v>
+      </c>
+      <c r="F17">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18">
+        <v>8</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
+      <c r="D18">
+        <v>6</v>
+      </c>
+      <c r="E18">
+        <v>6</v>
+      </c>
+      <c r="F18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19">
+        <v>6</v>
+      </c>
+      <c r="C19">
+        <v>6</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="F19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20">
+        <v>10</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21">
+        <v>6</v>
+      </c>
+      <c r="C21">
+        <v>10</v>
+      </c>
+      <c r="D21">
+        <v>9</v>
+      </c>
+      <c r="E21">
+        <v>10</v>
+      </c>
+      <c r="F21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <v>8</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DC8181E-EEAD-406A-BB8F-5A1C643475C3}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="B7:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -482,6 +1046,40 @@
         <v>8</v>
       </c>
     </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>15</v>
+      </c>
+      <c r="C2">
+        <v>20</v>
+      </c>
+      <c r="D2">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>8000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>